<commit_message>
Updates to timeline and clients, additon of multiple logos and updated xlsx
</commit_message>
<xml_diff>
--- a/src/resources/files/client_list.xlsb.xlsx
+++ b/src/resources/files/client_list.xlsb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="203">
   <si>
     <t xml:space="preserve">client_id</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">client_end_date</t>
   </si>
   <si>
+    <t xml:space="preserve">client_primary_technology</t>
+  </si>
+  <si>
     <t xml:space="preserve">PowerSchool (Formerly SunGuard)</t>
   </si>
   <si>
@@ -61,7 +64,7 @@
     <t xml:space="preserve">A C#.Net client of Eagle Creek that primary responsibility was to develop, enhance, and maintain the core functionality of their IEPPLUS 5 product. This entailed updating the application and modifying the layout and UI in T4 templated in .Net. It also included modifying and updating multiple Cristal Reports and batch jobs.</t>
   </si>
   <si>
-    <t xml:space="preserve">SQL Server, MS Visual Studio, Web Development, ASP.NET, C#, Crystal Reports, UI Templates, Team Foundation Server, HTML</t>
+    <t xml:space="preserve">SQL Server, MS Visual Studio, Web Development, ASP.NET, C#, Crystal Reports, UI Templates, Team Foundation Server, HTML, Jira</t>
   </si>
   <si>
     <t xml:space="preserve">power-school-logo</t>
@@ -73,6 +76,9 @@
     <t xml:space="preserve">2017-08-01</t>
   </si>
   <si>
+    <t xml:space="preserve">.Net</t>
+  </si>
+  <si>
     <t xml:space="preserve">PointIt</t>
   </si>
   <si>
@@ -85,7 +91,7 @@
     <t xml:space="preserve">Web Development, Marketing, HTML, SEO, Marketo, Salesforce</t>
   </si>
   <si>
-    <t xml:space="preserve">null</t>
+    <t xml:space="preserve">pointit_logo</t>
   </si>
   <si>
     <t xml:space="preserve">2015-04-01</t>
@@ -94,10 +100,16 @@
     <t xml:space="preserve">2017-05-01</t>
   </si>
   <si>
+    <t xml:space="preserve">Marketo</t>
+  </si>
+  <si>
     <t xml:space="preserve">8x8</t>
   </si>
   <si>
-    <t xml:space="preserve">A Marketo and Salesforce client of Eagle Creek that required the creation of multiple regional workspaces for North America and the United Kingdom. Configuartion for multiple regions and brands marketing and sales pipelines for leads.</t>
+    <t xml:space="preserve">A Marketo and Salesforce client of Eagle Creek that required the creation of multiple regional workspaces for North America and the United Kingdom. Configuration for multiple regions and brands marketing and sales pipelines for leads.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8x8_logo</t>
   </si>
   <si>
     <t xml:space="preserve">2015-02-01</t>
@@ -109,7 +121,7 @@
     <t xml:space="preserve">A Salesforce client of Eagle Creek that wanted to create a custom VisualForce site for their InnovationLink initiative. Utilizing VisualForce frontend and Apex backend we were able to create an HTML5 featured site with custom image cropping, dynamic YouTube video embedding and custom drop down menus for a custom experience for multiple user tiers.</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Development, Salesforce, VisualForce, Apex, HTML, Javascript, jQuery, LESS, CSS, Eclipse</t>
+    <t xml:space="preserve">Web Development, Salesforce, VisualForce, Apex, HTML, JavaScript, jQuery, LESS, CSS, Eclipse</t>
   </si>
   <si>
     <t xml:space="preserve">hca_healthcare_logo</t>
@@ -118,6 +130,9 @@
     <t xml:space="preserve">2016-02-01</t>
   </si>
   <si>
+    <t xml:space="preserve">Salesforce</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liverail</t>
   </si>
   <si>
@@ -127,6 +142,9 @@
     <t xml:space="preserve">Web Development, Marketing, Javascript, Marketo</t>
   </si>
   <si>
+    <t xml:space="preserve">liverail_logo</t>
+  </si>
+  <si>
     <t xml:space="preserve">2015-06-01</t>
   </si>
   <si>
@@ -136,7 +154,10 @@
     <t xml:space="preserve">A .Net client of Eagle Creek that needed an Asset Publisher a C# WCF to connect to local image storage using a PhotoManager service classes to get/post images that was exposed to AJAX and a FamilyManager service classes to get/post XML data sets.</t>
   </si>
   <si>
-    <t xml:space="preserve">SQL Server, MS Visual Studio, ASP.NET, C#</t>
+    <t xml:space="preserve">SQL Server, MS Visual Studio, ASP.NET, C#, SQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lifetouch2</t>
   </si>
   <si>
     <t xml:space="preserve">2016-05-01</t>
@@ -154,6 +175,9 @@
     <t xml:space="preserve">Web Development, Marketing, HTML, SEO, Marketo</t>
   </si>
   <si>
+    <t xml:space="preserve">skona_logo</t>
+  </si>
+  <si>
     <t xml:space="preserve">2014-05-01</t>
   </si>
   <si>
@@ -166,7 +190,7 @@
     <t xml:space="preserve">The State of Arizona Enterprise Procurement Services was a Drupal/PHP client that required on demand excel spreadsheets of CES, LAUS, &amp; QCEW tables that I provided a responsive UI with dynamic drop downs and modal spinner during data retrieval while the PHP backend retrieved the data and processed the excel download.</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Development, HTML, Javascript, jQuery, CSS, PHP, Eclipse</t>
+    <t xml:space="preserve">Web Development, HTML, JavaScript, jQuery, CSS, PHP, Eclipse</t>
   </si>
   <si>
     <t xml:space="preserve">state_of_arizona</t>
@@ -178,43 +202,517 @@
     <t xml:space="preserve">2016-04-01</t>
   </si>
   <si>
+    <t xml:space="preserve">Drupal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State of Arizona – DES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The State of Arizona Department of Economic Security was a Drupal client of Eagle Creek that required a Drupal 7 to 9/10 site migration. This required duplicating all existing pages from the current Drupal 7 site and migrating all data and data structures to the new Drupal 9/10 site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Development, HTML, Javascript, jQuery, CSS, SCSS, Drupal, PHP, Twig Templates, VSCode, Google Docs, Git/GitHub, Pantheon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-08-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eagle Creek an Eviden Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eagle Creek is a Minnesota based U.S. technology and management consulting company that  developed the industry’s first U.S. Onshore model as an alternative to offshore. With this employer I served as a Frontend UI specialist developing custom responsive UIs in various platforms Marketo Emails and Landing Pages, Salesforce Visualforce pages, Drupal 6/7/9/10, VB &amp; C# .Net full stack developer including Angular and Reactjs Technologies as well and a Fullstack building services and store procedures and optimizing queries in SQL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Development, HTML, JavaScript, jQuery, CSS, VB.Net, C#.Net, ASP.Net, Entity Framework, LINQ, SQL, T-SQL, MySQL, Oracle, Jira, AWS, React, Angular, JSP,  VisualForce Pages, ColdFusion, Git/GitHub, PHP, Java Servlets, RESTful Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eagle-Creek-logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eagle Creek is a Minnesota based U.S. technology and management consulting company that  developed the industry’s first U.S. Onshore model as an alternative to offshore. With this employer I was the lead Marketo expert that would provide Marketo Administration support, build custom templated Marketing Lifecycle programs and Salesforce integration. Custom integration with client sites through Marketo Munchkin code and campaigns. Automated email campaigns, progressive forms for whitepapers and even video editing and YouTube account administration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marketo, Salesforce, Web Development, HTML, JavaScript, jQuery, CSS, YouTube, Final Cut Pro, Adobe Illustrator CS6, Adobe Photoshop CS6, iMovie</t>
+  </si>
+  <si>
     <t xml:space="preserve">State of Arizona - DPS</t>
   </si>
   <si>
     <t xml:space="preserve">The State of Arizona Department of Public Safety Recruitment was a Drupal client of Eagle Creek that during a Drupal 7 to 9/10 migration required more custom UI enhancements that needed custom Javascript and CSS beyond the default theme </t>
   </si>
   <si>
-    <t xml:space="preserve">Web Development, HTML, Javascript, jQuery, CSS, SCSS, Drupal, PHP, Twig Templates, VSCode, Git/GitHub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-06-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eagle Creek an Atos Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eagle Creek is a Minnesota based U.S. technology and management consulting company that  developed the industry’s first U.S. Onshore model as an alternative to offshore. With this employer I served as a Frontend UI specialist devloping custom responisve UIs in various platforms Marketo Emails and Landing Pages, Salesforce Visualforce pages, Drupal 6/7/9/10, VB &amp; C# .Net full stack developer including Angular and Reactjs Technologies as well and a Fullstack building services and store procedures and optimizing queries in SQL.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web Development, HTML, Javascript, jQuery, CSS, VB.Net, C#.Net, ASP.Net, Entity Framework, LINQ, SQL, T-SQL, MySQL, Oracle, Jira, AWS, React, Angular, JSP,  VisualForce Pages, ColdFusion, Git/GitHub, PHP, Java Servlets, RESTful Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013-10-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-04-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eagle Creek is a Minnesota based U.S. technology and management consulting company that  developed the industry’s first U.S. Onshore model as an alternative to offshore. With this employer I was the lead Marketo expert that would provide Marketo Administration support, build custom templated Marketing Lifecycle programs and Salesforce integration. Custom integration with client sites through Marketo Munchkin code and capmaigns. Automated email campaigns, progressive forms for whitepapers and even video editing and YouTube account administration.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marketo, Salesforce, Web Development, HTML, Javascript, jQuery, CSS, YouTube, Final Cut Pro, Adobe Illustrator CS6, Adobe Photoshop CS6, iMovie</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Web Development, HTML, JavaScript, jQuery, CSS, SCSS, Drupal, PHP, Twig Templates, VSCode, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Google Docs, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Git/GitHub, Pantheon</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State of Arizona – DOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The State of Arizona Department of Revenue was a Drupal client of Eagle Creek that required a Drupal 7 to 9/10 site migration. This required duplicating all existing pages from the current Drupal 7 site and migrating all data and data structures to the new Drupal 9/10 site.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Web Development, HTML, JavaScript, jQuery, CSS, SCSS, Drupal, PHP, Twig Templates, VSCode, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Google Docs,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Git/GitHub, Pantheon</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State of Arizona – OAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The State of Arizona Office of the Attorney General was a Drupal client of Eagle Creek that required a Drupal 7 to 9/10 site migration. This required duplicating all existing pages from the current Drupal 7 site and migrating all data and data structures to the new Drupal 9/10 site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-11-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSL Solutions, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A .Net client of Eagle Creek that we updated and revised legacy code for readability and serviceability and resolved a back log of bugs and issues in their Jira ticketing system. Developed a new set of custom controls for their XAML application.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sql Server, MS Visual Studio, Jira, ASP.Net, C#, JavaScript, HTML, CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bd_gsl_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creative MediaWorks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A .Net client of Eagle Creek that was updating their SpeakCore application product for their clients. While implementing new features and updates that were unique to many client environments I also worked through Asana ticketing of bugs and issues raise by clients. Client facing for multiple clients and received employee of the quarter for my performance. &lt;br/&gt;&lt;br/&gt;“Dan has provided services to our company for almost two years, and I can't say enough about the job he has done for us. He has been a great contributor for us and is a vital member of our team. He has a positive, up-beat personality, and everyone from our team has enjoyed working with him. He's a very talented developer and has done a great job with completing tickets for our platform. He's been interfacing directly with clients in our ticketing system and has done an excellent job communicating with them regarding questions he has and in answering their questions. Dan is a great addition to any team, and I highly recommend him.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server, MS Visual Studio, Web Development, ASP.NET, C#, Team Foundation Server, HTML, CSS, SQL, Asana, JavaScript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creative_mediaworks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-08-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-05-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KinderCare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KinderCare was a web application client for their OneCMS and Champions projects with Eagle Creek. These projects utilized AngularJS with .Net’s C# backend for their new extended day activity enrollments.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AngularJS, C#.Net, Enity Framework, SQL, T-SQL, HTML, CSS, JavaScript, Jira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">champions-logo_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marchex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Marketo client that we established a Marketo, Salesforce and RingLead data sync to prevent duplicate leads and complications of returning leads being flagged. Developed of marketing programs and events. Developed Nurture campaign, lead scoring and lead lifecycle model for marketing funnel to sales in Salesforce. Created custom branded HTML asset templates for responsive landing pages and emails for reuse by client. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Development, Marketing, HTML, SEO, Marketo, Salesforce, RingLead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marchex_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KinderCare initial startup of the Champions project that POC’d Angular and .Net in expansion beyond their Parent Portal application.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kinder_care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-09-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dealer Tire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A client of Eagle Creek that was behind schedule for UI development I was brought on to bring up to speed. Using LESS, Bootstrap, I was able to create the responsive UI and create custom JavaScript to integrate the Cold Fusion Templates with the existing site and complete the project on time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Development, HTML, JavaScript, jQuery, CSS, Less, Linux, Node.js, Cold Fusion, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dealer_tire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-12-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kasasa (formerly BancVue)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BancVue, now Kasasa, was a Marketo client of Eagle Creek that had multiple Marketo workspaces for their clients with more than a dozen banks transitioning to the Kasasa rewards branding for Kasasa: K360 and InControl Checking. Branded emails, landing pages were setup for each financial institutions’ workspace to automate email campaigns to target customers and convert them to the new rewards programs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Development, Marketing, HTML, SEO, Marketo, Jira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kasasa_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Career Arc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Marketo client that we created 4 different tokenized emails with 1 having A/B/C testing variants for 6 total emails to use in their automated email campaigns. Then setup the campaigns and added the token fields and trained the new admin to setup and edit the fields.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">careerarc_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cipher Cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Marketo client that needed responsive landing pages created with their own branding and progressive forms. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ciphercloud_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-07-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-08-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evolv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Marketo client that needed help integrating their own website with Marketo munchkin code to capture page visits and form submissions outside of landing pages on the Marketo platform.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evolv_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaspersky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Marketo client that requested custom responsive email templates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaspersky_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A long time Marketo client that Eagle Creek setup the Marketing lifecycle and automated email campaigns for each white paper and event for 2014 into 2015 until helping them migrate to HubSpot in March of 2015. HTML development for asset templates for emails and landing pages. Custom JavaScript and jQuery for site enhancements not native to Marketo at the time. On24 Webinar integration as well as updating their On24 emails with custom HTML over the plain text automated outbound emails. Edited image and videos for presentations that was then uploaded to a YouTube account created for Natera was also performed until a media content manager was added onto their team.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Development, Marketing, HTML, SEO, Marketo, Creative Suit 6, Adobe Illustrator, Adobe Photoshop, On24, jQuery, JavaScript, iMovie, Final Cut Pro, YouTube.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natera_logo_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-03-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nexenta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Marketo client that had created a new instance in Marketo that needed to combine the old and new instances into a single domain. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nexenta_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnitude Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A marketo client that had 3 subscriptions for Noetix, Kalido, and Magnitude brands. Imported programs across the subscriptions to consolidate into a single instance using workspaces for the brands to manage them. Updated HTML and JavaScript used in landing pages and emails for better UX and email client compatibility.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">magnitude_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-09-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLI Systems</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">A repeat Marketo client of Eagle Creek that required </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">DemandBase integration for client for Marketo and Saleforce instances. Also did </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HTML work for responsive emails and landing page templates built off their provided Catapult Works designs and later design updates. Created TDD and step by step user guides for editing template assets.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">slisystems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauce Labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Marketo and Salesforce client of Eagle Creek that required dashboards/reporting in Salesforce based on both the “referrer-Lead source” and the “asset/event-Campaign” that any leads or contacts with an opportunity role were a part of. This information is to be used to document Marketing-Sources-Pipeline and the Opportunity Influence of Marketing’s programs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saucelabs_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBM Advanstar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Salesforce and Marketo client. Created a POC and the TDD for Salesforce/Marketo integration for Event emailing. Developed email scripting data retrieval for Custom Objects from Salesforce for emails.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanstar-Logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A long time client of Eagle Creek. A project that was going to be UI enhancements to address issues with UX tickets created by customers. A .Net appication that utilized Vue.js, GraphQL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server, MS Visual Studio, ASP.NET, C#, VueJS, GraphQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">andover_companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benchmark Electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line assembly: laser power supplies, IBM Server packaging and shipping, communications devices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">benchmark_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-08-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Buy Geek Squad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full-time Advanced Repair Agent. Gold certified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geek_squad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008-08-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ShopKo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electronics retail sales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shopko_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2007-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GameStop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video game sales. Keyholder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gamestop_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2004-07-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Buy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail sales. Media, Home Theater, Appliances, Computers, Cellular, Ops.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bby_logo_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-03-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wendy’s Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shift manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wendys_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000-08-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fast Food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Open Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teen volunteer, team lead &amp; keyholder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k_villages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1996-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1999-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banyan Point Condominiums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Squarespace site for a condominium HOA. Assisted in rebuilding links, creating/editing and uploading assets to site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Development, HTML, Squarespace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banyan_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-09-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Squarespace</t>
   </si>
 </sst>
 </file>
@@ -225,7 +723,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -253,6 +751,26 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="aptos Narrow"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -298,7 +816,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -321,6 +839,22 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -446,15 +980,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="73.55"/>
@@ -462,6 +996,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,34 +1027,40 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,28 +1068,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,28 +1100,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,28 +1132,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,28 +1164,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,28 +1196,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,28 +1228,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,57 +1260,63 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>56</v>
+        <v>65</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,28 +1324,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>62</v>
+        <v>72</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,28 +1356,935 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="H13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="1" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="195.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>62</v>
+      <c r="B22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CSS for corrected footer positioning, made experience sort into descending order, updated logo.
</commit_message>
<xml_diff>
--- a/src/resources/files/client_list.xlsb.xlsx
+++ b/src/resources/files/client_list.xlsb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="204">
   <si>
     <t xml:space="preserve">client_id</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">client_primary_technology</t>
   </si>
   <si>
+    <t xml:space="preserve">client_of</t>
+  </si>
+  <si>
     <t xml:space="preserve">PowerSchool (Formerly SunGuard)</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
     <t xml:space="preserve">.Net</t>
   </si>
   <si>
+    <t xml:space="preserve">Eagle Creek an Eviden Business</t>
+  </si>
+  <si>
     <t xml:space="preserve">PointIt</t>
   </si>
   <si>
@@ -218,9 +224,6 @@
   </si>
   <si>
     <t xml:space="preserve">2023-08-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eagle Creek an Eviden Business</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -363,7 +366,7 @@
     <t xml:space="preserve">Creative MediaWorks</t>
   </si>
   <si>
-    <t xml:space="preserve">A .Net client of Eagle Creek that was updating their SpeakCore application product for their clients. While implementing new features and updates that were unique to many client environments I also worked through Asana ticketing of bugs and issues raise by clients. Client facing for multiple clients and received employee of the quarter for my performance. &lt;br/&gt;&lt;br/&gt;“Dan has provided services to our company for almost two years, and I can't say enough about the job he has done for us. He has been a great contributor for us and is a vital member of our team. He has a positive, up-beat personality, and everyone from our team has enjoyed working with him. He's a very talented developer and has done a great job with completing tickets for our platform. He's been interfacing directly with clients in our ticketing system and has done an excellent job communicating with them regarding questions he has and in answering their questions. Dan is a great addition to any team, and I highly recommend him.”</t>
+    <t xml:space="preserve">A .Net client of Eagle Creek that was updating their SpeakCore application product for their clients. While implementing new features and updates that were unique to many client environments I also worked through Asana ticketing of bugs and issues raise by clients. Client facing for multiple clients and received employee of the first quarter in 2021 for my performance. &lt;br/&gt;&lt;br/&gt;“Dan has provided services to our company for almost two years, and I can't say enough about the job he has done for us. He has been a great contributor for us and is a vital member of our team. He has a positive, up-beat personality, and everyone from our team has enjoyed working with him. He's a very talented developer and has done a great job with completing tickets for our platform. He's been interfacing directly with clients in our ticketing system and has done an excellent job communicating with them regarding questions he has and in answering their questions. Dan is a great addition to any team, and I highly recommend him.”</t>
   </si>
   <si>
     <t xml:space="preserve">SQL Server, MS Visual Studio, Web Development, ASP.NET, C#, Team Foundation Server, HTML, CSS, SQL, Asana, JavaScript</t>
@@ -682,7 +685,7 @@
     <t xml:space="preserve">Fast Food</t>
   </si>
   <si>
-    <t xml:space="preserve">The Open Table</t>
+    <t xml:space="preserve">The Open Table – 10,000 Villages</t>
   </si>
   <si>
     <t xml:space="preserve">Teen volunteer, team lead &amp; keyholder.</t>
@@ -706,7 +709,7 @@
     <t xml:space="preserve">Web Development, HTML, Squarespace</t>
   </si>
   <si>
-    <t xml:space="preserve">Banyan_logo</t>
+    <t xml:space="preserve">banyan_point_logo_2</t>
   </si>
   <si>
     <t xml:space="preserve">2025-09-01</t>
@@ -980,10 +983,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O16" activeCellId="0" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -997,6 +1000,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,37 +1034,43 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,31 +1078,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,31 +1113,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>26</v>
+      <c r="K4" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,31 +1148,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1164,31 +1183,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,31 +1218,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1228,31 +1253,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1260,31 +1288,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,31 +1323,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>60</v>
+      <c r="K10" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,31 +1358,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,31 +1390,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,31 +1422,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1420,31 +1457,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,31 +1492,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,31 +1527,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="195.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,31 +1562,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,31 +1597,34 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,31 +1632,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,31 +1667,34 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,31 +1702,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,31 +1737,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,31 +1772,34 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,31 +1807,34 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,31 +1842,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,31 +1877,34 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,31 +1912,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,31 +1947,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,31 +1982,34 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1932,31 +2017,34 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="I30" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1964,31 +2052,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1996,31 +2087,34 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,31 +2122,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2060,28 +2157,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,28 +2186,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2118,28 +2215,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="J36" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2147,28 +2244,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="J37" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,28 +2273,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="J38" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2205,28 +2302,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="J39" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,28 +2331,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,28 +2360,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated about page, added Cascade Slider and Modal enhancements
</commit_message>
<xml_diff>
--- a/src/resources/files/client_list.xlsb.xlsx
+++ b/src/resources/files/client_list.xlsb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="219">
   <si>
     <t xml:space="preserve">client_id</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">client_of</t>
   </si>
   <si>
+    <t xml:space="preserve">background_image</t>
+  </si>
+  <si>
     <t xml:space="preserve">PowerSchool (Formerly SunGuard)</t>
   </si>
   <si>
@@ -121,6 +124,9 @@
     <t xml:space="preserve">2015-02-01</t>
   </si>
   <si>
+    <t xml:space="preserve">8X8_Marketo_Admin.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">HCA</t>
   </si>
   <si>
@@ -139,6 +145,9 @@
     <t xml:space="preserve">Salesforce</t>
   </si>
   <si>
+    <t xml:space="preserve">HCA_InnovationHome_Chevron_and_Dropdowns.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liverail</t>
   </si>
   <si>
@@ -211,6 +220,9 @@
     <t xml:space="preserve">Drupal</t>
   </si>
   <si>
+    <t xml:space="preserve">AZ_EPS_excel_download.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">State of Arizona – DES</t>
   </si>
   <si>
@@ -245,6 +257,9 @@
   </si>
   <si>
     <t xml:space="preserve">Application Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eagle_Creek_Employees.png</t>
   </si>
   <si>
     <t xml:space="preserve">Eagle Creek is a Minnesota based U.S. technology and management consulting company that  developed the industry’s first U.S. Onshore model as an alternative to offshore. With this employer I was the lead Marketo expert that would provide Marketo Administration support, build custom templated Marketing Lifecycle programs and Salesforce integration. Custom integration with client sites through Marketo Munchkin code and campaigns. Automated email campaigns, progressive forms for whitepapers and even video editing and YouTube account administration.</t>
@@ -381,6 +396,9 @@
     <t xml:space="preserve">2021-05-01</t>
   </si>
   <si>
+    <t xml:space="preserve">Creative_MediaWorks_SpeakCore.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">KinderCare</t>
   </si>
   <si>
@@ -396,6 +414,9 @@
     <t xml:space="preserve">2017-10-01</t>
   </si>
   <si>
+    <t xml:space="preserve">Champions_Before_and_After_School_Programs.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marchex</t>
   </si>
   <si>
@@ -408,6 +429,9 @@
     <t xml:space="preserve">marchex_logo</t>
   </si>
   <si>
+    <t xml:space="preserve">marchex_bia_kelsey.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">KinderCare initial startup of the Champions project that POC’d Angular and .Net in expansion beyond their Parent Portal application.</t>
   </si>
   <si>
@@ -417,6 +441,9 @@
     <t xml:space="preserve">2016-09-01</t>
   </si>
   <si>
+    <t xml:space="preserve">CMS-30855_Before.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dealer Tire</t>
   </si>
   <si>
@@ -435,6 +462,9 @@
     <t xml:space="preserve">Java</t>
   </si>
   <si>
+    <t xml:space="preserve">dealer_tire_tread_input.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kasasa (formerly BancVue)</t>
   </si>
   <si>
@@ -447,6 +477,9 @@
     <t xml:space="preserve">kasasa_logo</t>
   </si>
   <si>
+    <t xml:space="preserve">Bankvue_Go_Live_Results_Marketing_Activities.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Career Arc</t>
   </si>
   <si>
@@ -471,6 +504,9 @@
     <t xml:space="preserve">2014-08-01</t>
   </si>
   <si>
+    <t xml:space="preserve">CipherCloud_Landing_Page.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Evolv</t>
   </si>
   <si>
@@ -492,7 +528,7 @@
     <t xml:space="preserve">Natera</t>
   </si>
   <si>
-    <t xml:space="preserve">A long time Marketo client that Eagle Creek setup the Marketing lifecycle and automated email campaigns for each white paper and event for 2014 into 2015 until helping them migrate to HubSpot in March of 2015. HTML development for asset templates for emails and landing pages. Custom JavaScript and jQuery for site enhancements not native to Marketo at the time. On24 Webinar integration as well as updating their On24 emails with custom HTML over the plain text automated outbound emails. Edited image and videos for presentations that was then uploaded to a YouTube account created for Natera was also performed until a media content manager was added onto their team.</t>
+    <t xml:space="preserve">A long time Marketo client that Eagle Creek setup the Marketing lifecycle and automated email campaigns for their Horizon, Anora, Panorama &amp; Spectrum brands. Setting up their registrations and progressive forms for their white papers and events until helping them migrate to HubSpot in March of 2015. HTML development for asset templates for emails and landing pages. Custom JavaScript and jQuery for site enhancements not native to Marketo at the time. On24 Webinar integration as well as updating their On24 emails with custom HTML over the plain text automated outbound emails. Edited image and videos for presentations that was then uploaded to a YouTube account created for Natera was also performed until a media content manager was added onto their team.</t>
   </si>
   <si>
     <t xml:space="preserve">Web Development, Marketing, HTML, SEO, Marketo, Creative Suit 6, Adobe Illustrator, Adobe Photoshop, On24, jQuery, JavaScript, iMovie, Final Cut Pro, YouTube.</t>
@@ -507,6 +543,9 @@
     <t xml:space="preserve">2015-03-01</t>
   </si>
   <si>
+    <t xml:space="preserve">Natera_Panorama_YouTube.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nexenta</t>
   </si>
   <si>
@@ -526,6 +565,9 @@
   </si>
   <si>
     <t xml:space="preserve">2014-09-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnitude_functioning_logic.png</t>
   </si>
   <si>
     <t xml:space="preserve">SLI Systems</t>
@@ -563,6 +605,9 @@
   </si>
   <si>
     <t xml:space="preserve">slisystems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLI_Direct Mailer_ 2015_MM_-_BZ.png</t>
   </si>
   <si>
     <t xml:space="preserve">Sauce Labs</t>
@@ -983,10 +1028,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O16" activeCellId="0" sqref="O16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1001,6 +1046,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="46.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,40 +1083,43 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,34 +1127,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,34 +1162,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1148,34 +1200,37 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1183,34 +1238,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,34 +1273,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,34 +1308,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1288,34 +1343,37 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1323,34 +1381,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1358,31 +1416,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1390,31 +1451,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="I12" s="4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,34 +1486,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1457,34 +1521,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1492,34 +1556,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1527,34 +1591,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="195.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,34 +1626,37 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,34 +1664,37 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="J18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,34 +1702,37 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1667,34 +1740,37 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1702,34 +1778,37 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1737,34 +1816,37 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,34 +1854,34 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1807,34 +1889,37 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1842,34 +1927,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,69 +1962,72 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1947,34 +2035,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,34 +2070,37 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2017,34 +2108,37 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2052,34 +2146,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2087,34 +2181,34 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2122,34 +2216,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2157,28 +2251,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2186,28 +2280,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2215,28 +2309,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2244,28 +2338,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2273,28 +2367,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2302,28 +2396,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2331,28 +2425,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2360,28 +2454,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed image issue for SLI and added image and social media icons to footer.
</commit_message>
<xml_diff>
--- a/src/resources/files/client_list.xlsb.xlsx
+++ b/src/resources/files/client_list.xlsb.xlsx
@@ -607,7 +607,7 @@
     <t xml:space="preserve">slisystems</t>
   </si>
   <si>
-    <t xml:space="preserve">SLI_Direct Mailer_ 2015_MM_-_BZ.png</t>
+    <t xml:space="preserve">SLI_Direct_Mailer_2015_MM_BZ.png</t>
   </si>
   <si>
     <t xml:space="preserve">Sauce Labs</t>
@@ -1030,8 +1030,8 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Reduce image and video size/compressions, updated Nav to close in mobile views to outside clicks, moved data fetch for clients xlsx to its own component.
</commit_message>
<xml_diff>
--- a/src/resources/files/client_list.xlsb.xlsx
+++ b/src/resources/files/client_list.xlsb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="226">
   <si>
     <t xml:space="preserve">client_id</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">background_image</t>
   </si>
   <si>
+    <t xml:space="preserve">client_feedback</t>
+  </si>
+  <si>
     <t xml:space="preserve">PowerSchool (Formerly SunGuard)</t>
   </si>
   <si>
@@ -112,6 +115,9 @@
     <t xml:space="preserve">Marketo</t>
   </si>
   <si>
+    <t xml:space="preserve">“Dan has been such a huge help to our team. His expertise helps us fill in the gaps and makes our email programs run smoothly.” - Madeline @ Point It</t>
+  </si>
+  <si>
     <t xml:space="preserve">8x8</t>
   </si>
   <si>
@@ -199,6 +205,9 @@
     <t xml:space="preserve">2014-06-01</t>
   </si>
   <si>
+    <t xml:space="preserve">skona_apigee_email_template.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">State of Arizona - EPS</t>
   </si>
   <si>
@@ -259,13 +268,22 @@
     <t xml:space="preserve">Application Development</t>
   </si>
   <si>
-    <t xml:space="preserve">Eagle_Creek_Employees.png</t>
+    <t xml:space="preserve">Eagle_Creek_Employees.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Dan is a multi-tasker who demonstrates the ability to write code, mentor others, converse with the client and help the team when required. Dan understands the technical side of the application he is working on and can provide various roles when asked.  Although Dan has a good grasp of the technologies he continuously demonstrates the desire to learn more expanding his skills. Moreover, Dan expresses a willingness to collaborate with others and is motivated to complete the task at hand regardless of his time commitment.” -Jeff B @ Eagle Creek</t>
   </si>
   <si>
     <t xml:space="preserve">Eagle Creek is a Minnesota based U.S. technology and management consulting company that  developed the industry’s first U.S. Onshore model as an alternative to offshore. With this employer I was the lead Marketo expert that would provide Marketo Administration support, build custom templated Marketing Lifecycle programs and Salesforce integration. Custom integration with client sites through Marketo Munchkin code and campaigns. Automated email campaigns, progressive forms for whitepapers and even video editing and YouTube account administration.</t>
   </si>
   <si>
     <t xml:space="preserve">Marketo, Salesforce, Web Development, HTML, JavaScript, jQuery, CSS, YouTube, Final Cut Pro, Adobe Illustrator CS6, Adobe Photoshop CS6, iMovie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eagle_Creek_Employees_2.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Dan is reliable both with attendance and providing effective services for his clients. Dan is motivated to complete the task at hand meeting deadlines regardless of the time commitment while achieving the quality standards necessary to be successful. Moreover, Dan organizes his tasks on projects, communicates the deliverable expectations and anticipates potential blockers in which he proactively tackles. Most importantly, Dan is a self starter requiring little guidance and oversight with a keen knack knowing when to escalate issues.” - Jeff B @ Eagle Creek</t>
   </si>
   <si>
     <t xml:space="preserve">State of Arizona - DPS</t>
@@ -397,6 +415,9 @@
   </si>
   <si>
     <t xml:space="preserve">Creative_MediaWorks_SpeakCore.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Dan has provided services to our company for almost two years, and I can't say enough about the job he has done for us. He has been a great contributor for us and is a vital member of our team. He has a positive, up-beat personality, and everyone from our team has enjoyed working with him. He's a very talented developer and has done a great job with completing tickets for our platform. He's been interfacing directly with clients in our ticketing system and has done an excellent job communicating with them regarding questions he has and in answering their questions. Dan is a great addition to any team, and I highly recommend him.” - Ryan @ Creative Media Works</t>
   </si>
   <si>
     <t xml:space="preserve">KinderCare</t>
@@ -864,7 +885,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -887,6 +908,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1028,10 +1053,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1047,6 +1072,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="46.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="60.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,40 +1112,43 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,34 +1156,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1162,37 +1194,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1200,37 +1232,37 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,34 +1270,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,34 +1305,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1308,34 +1340,37 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,37 +1378,37 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1381,104 +1416,110 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="J12" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="L12" s="3" t="s">
-        <v>79</v>
+        <v>86</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,34 +1527,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1521,34 +1562,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1556,34 +1597,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,34 +1632,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="195.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1626,37 +1667,40 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>102</v>
+        <v>15</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>106</v>
+        <v>112</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,37 +1708,37 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="J18" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1702,37 +1746,37 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>115</v>
+        <v>24</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,37 +1784,37 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>109</v>
+        <v>125</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,37 +1822,37 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,37 +1860,37 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,34 +1898,34 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>55</v>
+        <v>142</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,37 +1933,37 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>55</v>
+        <v>145</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,34 +1971,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>55</v>
+        <v>151</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,34 +2006,34 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="I26" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,37 +2041,37 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>158</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,34 +2079,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>55</v>
+        <v>164</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,37 +2114,37 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>55</v>
+        <v>167</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,37 +2152,37 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>25</v>
+        <v>172</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2146,34 +2190,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2181,34 +2225,34 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>25</v>
+        <v>179</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,34 +2260,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2251,28 +2295,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,28 +2324,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2309,28 +2353,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,28 +2382,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="J37" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,28 +2411,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,28 +2440,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,28 +2469,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2454,28 +2498,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a slider Carousel and testimonials to the About page and updated the Home page text. Organized the App.css into element sections
</commit_message>
<xml_diff>
--- a/src/resources/files/client_list.xlsb.xlsx
+++ b/src/resources/files/client_list.xlsb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="227">
   <si>
     <t xml:space="preserve">client_id</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">Marketo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PointIt_Marketo_screenshot.png</t>
   </si>
   <si>
     <t xml:space="preserve">“Dan has been such a huge help to our team. His expertise helps us fill in the gaps and makes our email programs run smoothly.” - Madeline @ Point It</t>
@@ -399,7 +402,7 @@
     <t xml:space="preserve">Creative MediaWorks</t>
   </si>
   <si>
-    <t xml:space="preserve">A .Net client of Eagle Creek that was updating their SpeakCore application product for their clients. While implementing new features and updates that were unique to many client environments I also worked through Asana ticketing of bugs and issues raise by clients. Client facing for multiple clients and received employee of the first quarter in 2021 for my performance. &lt;br/&gt;&lt;br/&gt;“Dan has provided services to our company for almost two years, and I can't say enough about the job he has done for us. He has been a great contributor for us and is a vital member of our team. He has a positive, up-beat personality, and everyone from our team has enjoyed working with him. He's a very talented developer and has done a great job with completing tickets for our platform. He's been interfacing directly with clients in our ticketing system and has done an excellent job communicating with them regarding questions he has and in answering their questions. Dan is a great addition to any team, and I highly recommend him.”</t>
+    <t xml:space="preserve">A .Net client of Eagle Creek that was updating their SpeakCore application product for their clients. While implementing new features and updates that were unique to many client environments I also worked through Asana ticketing of bugs and issues raise by clients. Client facing for multiple clients and received employee of the first quarter in 2021 for my performance.</t>
   </si>
   <si>
     <t xml:space="preserve">SQL Server, MS Visual Studio, Web Development, ASP.NET, C#, Team Foundation Server, HTML, CSS, SQL, Asana, JavaScript</t>
@@ -1055,8 +1058,8 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1185,8 +1188,11 @@
       <c r="K3" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="M3" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1194,7 +1200,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -1203,16 +1209,16 @@
         <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>28</v>
@@ -1224,7 +1230,7 @@
         <v>22</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,7 +1238,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -1241,28 +1247,28 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,7 +1276,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -1279,19 +1285,19 @@
         <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>30</v>
@@ -1305,7 +1311,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -1314,19 +1320,19 @@
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>21</v>
@@ -1340,7 +1346,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -1349,19 +1355,19 @@
         <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>30</v>
@@ -1370,7 +1376,7 @@
         <v>22</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,7 +1384,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -1387,28 +1393,28 @@
         <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,7 +1422,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -1425,22 +1431,22 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>22</v>
@@ -1454,34 +1460,34 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1492,34 +1498,34 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1527,7 +1533,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
@@ -1536,22 +1542,22 @@
         <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>22</v>
@@ -1562,7 +1568,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -1571,22 +1577,22 @@
         <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>22</v>
@@ -1597,7 +1603,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
@@ -1606,22 +1612,22 @@
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>22</v>
@@ -1632,7 +1638,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
@@ -1641,19 +1647,19 @@
         <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>21</v>
@@ -1662,12 +1668,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="195.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
@@ -1676,19 +1682,19 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>21</v>
@@ -1697,10 +1703,10 @@
         <v>22</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,7 +1714,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>
@@ -1717,19 +1723,19 @@
         <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>21</v>
@@ -1738,7 +1744,7 @@
         <v>22</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,7 +1752,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>14</v>
@@ -1755,16 +1761,16 @@
         <v>24</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>29</v>
@@ -1776,7 +1782,7 @@
         <v>22</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,7 +1790,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>14</v>
@@ -1793,16 +1799,16 @@
         <v>15</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>19</v>
@@ -1814,7 +1820,7 @@
         <v>22</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,7 +1828,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
@@ -1831,28 +1837,28 @@
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,7 +1866,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>14</v>
@@ -1869,19 +1875,19 @@
         <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>30</v>
@@ -1890,7 +1896,7 @@
         <v>22</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1898,7 +1904,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
@@ -1907,19 +1913,19 @@
         <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>30</v>
@@ -1933,7 +1939,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>14</v>
@@ -1942,19 +1948,19 @@
         <v>24</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>30</v>
@@ -1963,7 +1969,7 @@
         <v>22</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,7 +1977,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>14</v>
@@ -1980,19 +1986,19 @@
         <v>24</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>30</v>
@@ -2006,7 +2012,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>14</v>
@@ -2015,19 +2021,19 @@
         <v>24</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>30</v>
@@ -2041,7 +2047,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>14</v>
@@ -2050,19 +2056,19 @@
         <v>24</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>30</v>
@@ -2071,7 +2077,7 @@
         <v>22</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,7 +2085,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>14</v>
@@ -2088,19 +2094,19 @@
         <v>24</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>30</v>
@@ -2114,7 +2120,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>14</v>
@@ -2123,19 +2129,19 @@
         <v>24</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>30</v>
@@ -2144,7 +2150,7 @@
         <v>22</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2158,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>14</v>
@@ -2161,19 +2167,19 @@
         <v>24</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>30</v>
@@ -2182,7 +2188,7 @@
         <v>22</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2190,7 +2196,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>14</v>
@@ -2199,19 +2205,19 @@
         <v>24</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>30</v>
@@ -2225,7 +2231,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>14</v>
@@ -2234,16 +2240,16 @@
         <v>24</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>28</v>
@@ -2260,7 +2266,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>14</v>
@@ -2269,19 +2275,19 @@
         <v>15</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>21</v>
@@ -2295,28 +2301,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2324,28 +2330,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2353,28 +2359,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J36" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2382,28 +2388,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="J37" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2411,28 +2417,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="J38" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2440,28 +2446,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="J39" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,28 +2475,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2498,7 +2504,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>14</v>
@@ -2507,19 +2513,19 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Client update for experience page
</commit_message>
<xml_diff>
--- a/src/resources/files/client_list.xlsb.xlsx
+++ b/src/resources/files/client_list.xlsb.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Portfolio\src\resources\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F5E05D-6893-4195-AA90-371FEFC414EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5CBBCC-2C69-4468-97DC-A9389DA3933F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="231">
   <si>
     <t>client_id</t>
   </si>
@@ -774,9 +775,6 @@
     <t>Banyan Point Condominiums</t>
   </si>
   <si>
-    <t>A Squarespace site for a condominium HOA. Assisted in rebuilding links, creating/editing and uploading assets to site.</t>
-  </si>
-  <si>
     <t>Web Development, HTML, Squarespace</t>
   </si>
   <si>
@@ -790,6 +788,21 @@
   </si>
   <si>
     <t>The State of Arizona Office of the Auditor General was a Drupal client of Eagle Creek that required a Drupal 7 to 9/10 site migration. This required duplicating all existing pages from the current Drupal 7 site and migrating all data and data structures to the new Drupal 9/10 site.</t>
+  </si>
+  <si>
+    <t>A Squarespace site for a condominium HOA. Assisted in rebuilding links, creating/editing and uploading assets to their Squarespace site. Providing general technical support with PDF and Microsoft Office products.</t>
+  </si>
+  <si>
+    <t>Upwork &amp; Fiverr</t>
+  </si>
+  <si>
+    <t>Freelance</t>
+  </si>
+  <si>
+    <t>Freelance work from Marketing Automation integration support to Full-stack Code Reviews and optimizations and Security Audits.</t>
+  </si>
+  <si>
+    <t>Freelance Work</t>
   </si>
 </sst>
 </file>
@@ -853,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -870,6 +883,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1553,7 +1567,7 @@
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>91</v>
@@ -2440,7 +2454,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2454,19 +2468,45 @@
         <v>15</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" t="s">
         <v>222</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>223</v>
       </c>
-      <c r="H41" t="s">
+      <c r="J41" t="s">
         <v>224</v>
       </c>
-      <c r="J41" t="s">
-        <v>225</v>
+    </row>
+    <row r="42" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>227</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>228</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H42" s="8">
+        <v>45931</v>
+      </c>
+      <c r="J42" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing Excel date formating
</commit_message>
<xml_diff>
--- a/src/resources/files/client_list.xlsb.xlsx
+++ b/src/resources/files/client_list.xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Portfolio\src\resources\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5CBBCC-2C69-4468-97DC-A9389DA3933F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0A382E-D59F-4C6B-8BF7-BE2A2E2BA632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="233">
   <si>
     <t>client_id</t>
   </si>
@@ -803,6 +803,12 @@
   </si>
   <si>
     <t>Freelance Work</t>
+  </si>
+  <si>
+    <t>logo192</t>
+  </si>
+  <si>
+    <t>2025-10-01</t>
   </si>
 </sst>
 </file>
@@ -883,7 +889,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1013,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="E29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2502,8 +2508,11 @@
       <c r="F42" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H42" s="8">
-        <v>45931</v>
+      <c r="G42" t="s">
+        <v>231</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>232</v>
       </c>
       <c r="J42" t="s">
         <v>230</v>

</xml_diff>